<commit_message>
Refactor with COMM design
</commit_message>
<xml_diff>
--- a/mV_to_power_mapping - 20A - 200ohm.xlsx
+++ b/mV_to_power_mapping - 20A - 200ohm.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1681557865" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1681557865" showFormulas="1" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1681557865" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1681557865"/>
+      <pm:revision xmlns:pm="smNativeData" day="1681578501" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1681578501" showFormulas="1" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1681578501" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1681578501"/>
     </ext>
   </extLst>
 </workbook>
@@ -57,7 +57,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1681557865" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1681578501" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -73,7 +73,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1681557865" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1681578501" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -82,7 +82,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,19 +92,8 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1681557865" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -120,7 +109,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681557865"/>
+          <pm:border xmlns:pm="smNativeData" id="1681578501"/>
         </ext>
       </extLst>
     </border>
@@ -139,31 +128,12 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681557865">
+          <pm:border xmlns:pm="smNativeData" id="1681578501">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681557865"/>
         </ext>
       </extLst>
     </border>
@@ -185,7 +155,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1681557865" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1681578501" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -231,7 +201,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="100">
+                  <a:defRPr lang="en-us" sz="1170" b="0" i="0" u="none" strike="noStrike" kern="100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -249,35 +219,53 @@
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
+            <c:name>Poly-3</c:name>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
             <c:intercept val="0.000000"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.056000E-01"/>
-                  <c:y val="3.972000E-01"/>
+                  <c:x val="-3.587000E-01"/>
+                  <c:y val="-2.520000E-02"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="1"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-              </c:spPr>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="100">
+                    <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike">
                       <a:solidFill>
                         <a:srgbClr val="000000"/>
                       </a:solidFill>
-                      <a:latin typeface="Arial" charset="0"/>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:name>exponential</c:name>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
                 </a:p>
@@ -475,7 +463,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-us" sz="2510" b="0" i="0" u="none" strike="noStrike" kern="100">
+        <a:defRPr lang="en-us" sz="2935" b="0" i="0" u="none" strike="noStrike" kern="100">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -486,7 +474,7 @@
   </c:txPr>
   <c:extLst>
     <c:ext xmlns:sm="smo" uri="smo">
-      <sm:colorScheme xmlns:sm="smo" id="1681557865" val="7"/>
+      <sm:colorScheme xmlns:sm="smo" id="1681578501" val="7"/>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -502,10 +490,10 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>132715</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>120015</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -786,7 +774,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -971,7 +959,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1681557865" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1681578501" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -980,17 +968,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1681557865" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1681557865" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1681557865" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1681557865" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1681578501" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1681578501" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1681578501" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1681578501" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1681557865" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1681578501" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>